<commit_message>
added save-state from previous weights
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.479586869424565</v>
+        <v>6.268868452723979</v>
       </c>
       <c r="C2" t="n">
         <v>1000</v>
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4740469572437137</v>
+        <v>-0.4033703316514688</v>
       </c>
       <c r="C3" t="n">
         <v>1000</v>
@@ -472,20 +472,9 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6327770874505945</v>
+        <v>-2.676184643176573</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.9198507692954556</v>
-      </c>
-      <c r="C5" t="n">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed counter of epochs on results.xlsx
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>6.268868452723979</v>
+        <v>6.543317604821462</v>
       </c>
       <c r="C2" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4033703316514688</v>
+        <v>-0.4712688683213287</v>
       </c>
       <c r="C3" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.676184643176573</v>
+        <v>-2.996506018092723</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>